<commit_message>
deleted copied repo folders
</commit_message>
<xml_diff>
--- a/ch17/TaxonomiesMapping.xlsx
+++ b/ch17/TaxonomiesMapping.xlsx
@@ -19,10 +19,10 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1719806593" val="1210" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1719806593" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1719806593" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1719806593"/>
+      <pm:revision xmlns:pm="smNativeData" day="1719796191" val="1210" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1719796191" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1719796191" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1719796191"/>
     </ext>
   </extLst>
 </workbook>
@@ -837,7 +837,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1719806593" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1719796191" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -852,7 +852,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1719806593" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1719796191" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -868,7 +868,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1719806593" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1719796191" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default" i="1"/>
             <pm:cs face="Basic Roman" sz="200" lang="default" i="1"/>
             <pm:ea face="Basic Roman" sz="200" lang="default" i="1"/>
@@ -884,7 +884,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1719806593" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1719796191" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default" weight="bold"/>
             <pm:cs face="Basic Roman" sz="200" lang="default" weight="bold"/>
             <pm:ea face="Basic Roman" sz="200" lang="default" weight="bold"/>
@@ -900,7 +900,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1719806593" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1719796191" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default" i="1"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -916,7 +916,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1719806593" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1719796191" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default" weight="bold"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -925,7 +925,7 @@
       </extLst>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -941,13 +941,24 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1719806593" type="1" fgLvl="100" fgClr="00000000" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1719796191" type="1" fgLvl="100" fgClr="00000000" bgLvl="100" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1719796191" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left style="none">
         <color rgb="FF000000"/>
@@ -963,7 +974,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1719806593"/>
+          <pm:border xmlns:pm="smNativeData" id="1719796191"/>
         </ext>
       </extLst>
     </border>
@@ -982,7 +993,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1719806593">
+          <pm:border xmlns:pm="smNativeData" id="1719796191">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -1006,7 +1017,26 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1719806593"/>
+          <pm:border xmlns:pm="smNativeData" id="1719796191"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1719796191"/>
         </ext>
       </extLst>
     </border>
@@ -1054,7 +1084,7 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1719806593" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1719796191" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
     </ext>
@@ -1355,7 +1385,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
@@ -1969,7 +1999,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1719806593" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1719796191" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1978,14 +2008,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1719806593" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1719806593" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1719796191" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1719796191" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1719806593" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1719796191" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -2260,7 +2290,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1719806593" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1719796191" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -2269,8 +2299,8 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1719806593" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1719806593" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1719796191" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1719796191" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
@@ -2279,7 +2309,7 @@
   </tableParts>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1719806593" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1719796191" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -2547,7 +2577,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1719806593" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1719796191" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -2556,8 +2586,8 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1719806593" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1719806593" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1719796191" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1719796191" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
@@ -2566,7 +2596,7 @@
   </tableParts>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1719806593" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1719796191" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -2833,7 +2863,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1719806593" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1719796191" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -2842,8 +2872,8 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1719806593" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1719806593" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1719796191" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1719796191" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
@@ -2852,7 +2882,7 @@
   </tableParts>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1719806593" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1719796191" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>